<commit_message>
done project 4. commit before 1st submission
</commit_message>
<xml_diff>
--- a/project4/times.xlsx
+++ b/project4/times.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="360" windowWidth="25600" windowHeight="16640" tabRatio="500"/>
+    <workbookView xWindow="4620" yWindow="0" windowWidth="23080" windowHeight="16920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="5">
   <si>
     <t>No. of processes</t>
   </si>
@@ -31,6 +31,9 @@
   </si>
   <si>
     <t>DNA MPI kmeans</t>
+  </si>
+  <si>
+    <t>Seq</t>
   </si>
 </sst>
 </file>
@@ -79,8 +82,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="9">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -93,15 +100,19 @@
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -169,10 +180,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$13</c:f>
+              <c:f>Sheet1!$C$19:$C$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -202,45 +213,75 @@
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$4:$D$13</c:f>
+              <c:f>Sheet1!$D$19:$D$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>55.7667448521</c:v>
+                  <c:v>14.7617080212</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>33.9277999401</c:v>
+                  <c:v>7.93413805962</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>23.110352993</c:v>
+                  <c:v>5.39798283577</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.3448140621</c:v>
+                  <c:v>4.26211905479</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.4267590046</c:v>
+                  <c:v>3.59704089165</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17.8916881084</c:v>
+                  <c:v>3.19927883148</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>16.8964538574</c:v>
+                  <c:v>2.92680120468</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>15.8140158653</c:v>
+                  <c:v>2.69825792313</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>14.6147069931</c:v>
+                  <c:v>2.5080280304</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>16.0313980579</c:v>
+                  <c:v>2.42210292816</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.39634394646</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.3590221405</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.28407001495</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.30212402344</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.34637403488</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -255,11 +296,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="733948568"/>
-        <c:axId val="733582376"/>
+        <c:axId val="607416456"/>
+        <c:axId val="556967320"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="733948568"/>
+        <c:axId val="607416456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -288,12 +329,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733582376"/>
+        <c:crossAx val="556967320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="733582376"/>
+        <c:axId val="556967320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -323,7 +364,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733948568"/>
+        <c:crossAx val="607416456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -400,10 +441,10 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$F$4:$F$9</c:f>
+              <c:f>Sheet1!$F$19:$F$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -421,33 +462,87 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>30.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$G$4:$G$9</c:f>
+              <c:f>Sheet1!$G$19:$G$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>24.3866009712</c:v>
+                  <c:v>11.9622499943</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15.3986680508</c:v>
+                  <c:v>6.64000320435</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11.7147271633</c:v>
+                  <c:v>4.98771691322</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.62190318108</c:v>
+                  <c:v>3.93734312057</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.84342694283</c:v>
+                  <c:v>3.43249583244</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.07878708839</c:v>
+                  <c:v>3.05401015282</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.8865480423</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.67045617104</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.53081202507</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.40444207191</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.34941601753</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.30453085899</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.30475902557</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.32808709145</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.36258912086</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -462,11 +557,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="733935032"/>
-        <c:axId val="733638824"/>
+        <c:axId val="141192952"/>
+        <c:axId val="141222328"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="733935032"/>
+        <c:axId val="141192952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,12 +590,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733638824"/>
+        <c:crossAx val="141222328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="733638824"/>
+        <c:axId val="141222328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -530,7 +625,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="733935032"/>
+        <c:crossAx val="141192952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -934,10 +1029,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:G13"/>
+  <dimension ref="C2:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1078,6 +1173,252 @@
       </c>
       <c r="D13">
         <v>16.031398057899999</v>
+      </c>
+    </row>
+    <row r="15" spans="3:7">
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15">
+        <v>24.678992986699999</v>
+      </c>
+      <c r="F15" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15">
+        <v>20.897022008899999</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7">
+      <c r="C17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7">
+      <c r="C18" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19">
+        <v>14.7617080212</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="G19">
+        <v>11.9622499943</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7">
+      <c r="C20">
+        <v>4</v>
+      </c>
+      <c r="D20">
+        <v>7.9341380596200004</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>6.6400032043500001</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7">
+      <c r="C21">
+        <v>6</v>
+      </c>
+      <c r="D21">
+        <v>5.3979828357699997</v>
+      </c>
+      <c r="F21">
+        <v>6</v>
+      </c>
+      <c r="G21">
+        <v>4.9877169132199999</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7">
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>4.2621190547900003</v>
+      </c>
+      <c r="F22">
+        <v>8</v>
+      </c>
+      <c r="G22">
+        <v>3.93734312057</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7">
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>3.5970408916499998</v>
+      </c>
+      <c r="F23">
+        <v>10</v>
+      </c>
+      <c r="G23">
+        <v>3.4324958324399999</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7">
+      <c r="C24">
+        <v>12</v>
+      </c>
+      <c r="D24">
+        <v>3.19927883148</v>
+      </c>
+      <c r="F24">
+        <v>12</v>
+      </c>
+      <c r="G24">
+        <v>3.0540101528200001</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7">
+      <c r="C25">
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>2.9268012046799998</v>
+      </c>
+      <c r="F25">
+        <v>14</v>
+      </c>
+      <c r="G25">
+        <v>2.8865480422999998</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7">
+      <c r="C26">
+        <v>16</v>
+      </c>
+      <c r="D26">
+        <v>2.6982579231299999</v>
+      </c>
+      <c r="F26">
+        <v>16</v>
+      </c>
+      <c r="G26">
+        <v>2.6704561710400001</v>
+      </c>
+    </row>
+    <row r="27" spans="3:7">
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>2.5080280304000002</v>
+      </c>
+      <c r="F27">
+        <v>18</v>
+      </c>
+      <c r="G27">
+        <v>2.5308120250699999</v>
+      </c>
+    </row>
+    <row r="28" spans="3:7">
+      <c r="C28">
+        <v>20</v>
+      </c>
+      <c r="D28">
+        <v>2.4221029281600002</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+      <c r="G28">
+        <v>2.4044420719100001</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7">
+      <c r="C29">
+        <v>22</v>
+      </c>
+      <c r="D29">
+        <v>2.39634394646</v>
+      </c>
+      <c r="F29">
+        <v>22</v>
+      </c>
+      <c r="G29">
+        <v>2.3494160175299998</v>
+      </c>
+    </row>
+    <row r="30" spans="3:7">
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30">
+        <v>2.3590221405</v>
+      </c>
+      <c r="F30">
+        <v>24</v>
+      </c>
+      <c r="G30">
+        <v>2.3045308589900002</v>
+      </c>
+    </row>
+    <row r="31" spans="3:7">
+      <c r="C31">
+        <v>26</v>
+      </c>
+      <c r="D31">
+        <v>2.2840700149500002</v>
+      </c>
+      <c r="F31">
+        <v>26</v>
+      </c>
+      <c r="G31">
+        <v>2.3047590255700001</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7">
+      <c r="C32">
+        <v>28</v>
+      </c>
+      <c r="D32">
+        <v>2.3021240234399998</v>
+      </c>
+      <c r="F32">
+        <v>28</v>
+      </c>
+      <c r="G32">
+        <v>2.32808709145</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7">
+      <c r="C33">
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <v>2.3463740348800002</v>
+      </c>
+      <c r="F33">
+        <v>30</v>
+      </c>
+      <c r="G33">
+        <v>2.3625891208600001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>